<commit_message>
v 0.19.1.29 fix import GroupInRows
</commit_message>
<xml_diff>
--- a/demos/imports/xls/xls/GroupInRows.xlsx
+++ b/demos/imports/xls/xls/GroupInRows.xlsx
@@ -455,7 +455,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,18 +472,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF5983B0"/>
         <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEC9BA4"/>
-        <bgColor rgb="FFFF8080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB47804"/>
-        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -528,7 +516,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -565,14 +553,6 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,7 +575,7 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFB47804"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB4C7DC"/>
@@ -621,7 +601,7 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFEC9BA4"/>
+      <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
@@ -652,8 +632,8 @@
   </sheetPr>
   <dimension ref="A3:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1141,19 +1121,19 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="n">
@@ -1351,19 +1331,19 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">

</xml_diff>